<commit_message>
wip: wires back to 1x1 lol
</commit_message>
<xml_diff>
--- a/assets/grids.xlsx
+++ b/assets/grids.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\link-builder\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C369B78A-553D-4BC7-97CA-5CADCEF4985C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="grids" sheetId="1" r:id="rId1"/>
+    <sheet name="wire" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>-90 = down</t>
   </si>
@@ -33,12 +35,57 @@
   </si>
   <si>
     <t>xy</t>
+  </si>
+  <si>
+    <t>rotation
+-270
+90</t>
+  </si>
+  <si>
+    <t>rotation
+0
+360</t>
+  </si>
+  <si>
+    <t>rotation
+-90
+270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotation
+-180
+180
+</t>
+  </si>
+  <si>
+    <t>right = 0
+down = 0
+left = 1
+up = 1</t>
+  </si>
+  <si>
+    <t>right = 1
+down = 0
+left = 0
+up = 1</t>
+  </si>
+  <si>
+    <t>right = 0
+down = 1
+left = 1
+up = 0</t>
+  </si>
+  <si>
+    <t>right = 1
+down = 1
+left = 0
+up = 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -48,12 +95,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCC5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -83,16 +136,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDCC5FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -102,6 +174,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>11208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7239</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC1A907-3CD3-4D64-A90A-72A68DB2D850}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4941795" y="1232649"/>
+          <a:ext cx="6159268" cy="2454087"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,16 +487,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D7:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="22" width="4.5703125" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="4:18" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -386,7 +508,7 @@
       <c r="N8">
         <v>1</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="3">
         <v>2</v>
       </c>
       <c r="P8">
@@ -404,9 +526,7 @@
         <v>2</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="1">
-        <v>-2</v>
-      </c>
+      <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
@@ -439,20 +559,17 @@
       <c r="I11" s="1">
         <v>-2</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="3">
         <v>2</v>
       </c>
-      <c r="M11" s="1">
-        <v>-2</v>
-      </c>
+      <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P11" s="1"/>
-      <c r="Q11" s="1">
-        <v>-2</v>
-      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="3"/>
     </row>
     <row r="12" spans="4:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12">
@@ -504,7 +621,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="O14" s="4"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -531,4 +648,86 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14FF964-5053-479B-91D4-E587C49DDECF}">
+  <dimension ref="D3:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="96" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="4:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="4:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="4:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="4:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+      <c r="E6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="4:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
wip: fixing wire ports
</commit_message>
<xml_diff>
--- a/assets/grids.xlsx
+++ b/assets/grids.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\link-builder\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rstenson\Documents\GameMakerStudio2\link-builder\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7467CF6A-BD69-4866-95FD-96F62568A608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="grids" sheetId="1" r:id="rId1"/>
@@ -129,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,9 +209,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -221,6 +217,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D7:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -719,7 +718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14FF964-5053-479B-91D4-E587C49DDECF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:J8"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -801,11 +800,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8339B6B-4684-4744-9157-13BB49D2FAE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H8:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +857,7 @@
         <v>11</v>
       </c>
       <c r="O9" s="9"/>
-      <c r="S9" s="11" t="s">
+      <c r="S9" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -869,15 +868,15 @@
       <c r="I10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
       <c r="O10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="11"/>
+      <c r="S10" s="14"/>
     </row>
     <row r="11" spans="8:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H11">
@@ -886,11 +885,11 @@
       <c r="I11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
       <c r="O11" s="9" t="s">
         <v>11</v>
       </c>
@@ -905,11 +904,11 @@
       <c r="I12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
       <c r="O12" s="9" t="s">
         <v>11</v>
       </c>
@@ -924,11 +923,11 @@
       <c r="I13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
       <c r="O13" s="9" t="s">
         <v>11</v>
       </c>
@@ -943,11 +942,11 @@
       <c r="I14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
       <c r="O14" s="9" t="s">
         <v>11</v>
       </c>
@@ -978,25 +977,25 @@
       <c r="O15" s="9"/>
     </row>
     <row r="17" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S17" s="13"/>
+      <c r="S17" s="12"/>
     </row>
     <row r="18" spans="19:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S18" s="14" t="s">
+      <c r="S18" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="19:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S19" s="14" t="s">
+      <c r="S19" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="19:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S20" s="14" t="s">
+      <c r="S20" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="19:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S21" s="14" t="s">
+      <c r="S21" s="13" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>